<commit_message>
Placed Ring of Piety in proper order
</commit_message>
<xml_diff>
--- a/Vanilla_Shaman.xlsx
+++ b/Vanilla_Shaman.xlsx
@@ -10798,28 +10798,30 @@
       <c r="Q201" s="28"/>
     </row>
     <row r="202" spans="1:17" ht="15.6">
-      <c r="A202" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B202" s="63" t="s">
-        <v>481</v>
+      <c r="A202" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="B202" s="102" t="s">
+        <v>567</v>
       </c>
       <c r="C202" s="39" t="s">
         <v>158</v>
       </c>
       <c r="D202" s="19">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="E202" s="19">
-        <v>12</v>
-      </c>
-      <c r="F202" s="19"/>
+        <v>10</v>
+      </c>
+      <c r="F202" s="19">
+        <v>4</v>
+      </c>
       <c r="G202" s="21">
-        <f t="shared" ref="G202:G225" si="15">(E202/5)+(F202)+(D202/7)</f>
-        <v>8.9714285714285715</v>
+        <f>(E202/5)+(F202)+(D202/7)</f>
+        <v>9.1428571428571423</v>
       </c>
       <c r="H202" s="19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I202" s="19"/>
       <c r="J202" s="19"/>
@@ -10832,28 +10834,28 @@
       <c r="Q202" s="28"/>
     </row>
     <row r="203" spans="1:17" ht="15.6">
-      <c r="A203" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B203" s="65" t="s">
-        <v>391</v>
+      <c r="A203" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B203" s="63" t="s">
+        <v>481</v>
       </c>
       <c r="C203" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="D203" s="19"/>
+      <c r="D203" s="19">
+        <v>46</v>
+      </c>
       <c r="E203" s="19">
-        <v>10</v>
-      </c>
-      <c r="F203" s="19">
-        <v>6</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F203" s="19"/>
       <c r="G203" s="21">
-        <f>(E203/5)+(F203)+(D203/7)</f>
-        <v>8</v>
+        <f t="shared" ref="G203:G225" si="15">(E203/5)+(F203)+(D203/7)</f>
+        <v>8.9714285714285715</v>
       </c>
       <c r="H203" s="19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I203" s="19"/>
       <c r="J203" s="19"/>
@@ -10867,10 +10869,10 @@
     </row>
     <row r="204" spans="1:17" ht="15.6">
       <c r="A204" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B204" s="64" t="s">
-        <v>430</v>
+        <v>185</v>
+      </c>
+      <c r="B204" s="65" t="s">
+        <v>391</v>
       </c>
       <c r="C204" s="39" t="s">
         <v>158</v>
@@ -10883,10 +10885,12 @@
         <v>6</v>
       </c>
       <c r="G204" s="21">
-        <f t="shared" si="15"/>
+        <f>(E204/5)+(F204)+(D204/7)</f>
         <v>8</v>
       </c>
-      <c r="H204" s="19"/>
+      <c r="H204" s="19">
+        <v>8</v>
+      </c>
       <c r="I204" s="19"/>
       <c r="J204" s="19"/>
       <c r="K204" s="19"/>
@@ -10899,24 +10903,24 @@
     </row>
     <row r="205" spans="1:17" ht="15.6">
       <c r="A205" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B205" s="65" t="s">
-        <v>484</v>
+        <v>38</v>
+      </c>
+      <c r="B205" s="64" t="s">
+        <v>430</v>
       </c>
       <c r="C205" s="39" t="s">
         <v>158</v>
       </c>
       <c r="D205" s="19"/>
       <c r="E205" s="19">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F205" s="19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G205" s="21">
-        <f>(E205/5)+(F205)+(D205/7)</f>
-        <v>6.6</v>
+        <f t="shared" si="15"/>
+        <v>8</v>
       </c>
       <c r="H205" s="19"/>
       <c r="I205" s="19"/>
@@ -10931,29 +10935,27 @@
     </row>
     <row r="206" spans="1:17" ht="15.6">
       <c r="A206" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B206" s="65" t="s">
-        <v>449</v>
+        <v>484</v>
       </c>
       <c r="C206" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="D206" s="19">
-        <v>29</v>
-      </c>
+      <c r="D206" s="19"/>
       <c r="E206" s="19">
-        <v>12</v>
-      </c>
-      <c r="F206" s="19"/>
+        <v>13</v>
+      </c>
+      <c r="F206" s="19">
+        <v>4</v>
+      </c>
       <c r="G206" s="21">
         <f>(E206/5)+(F206)+(D206/7)</f>
-        <v>6.5428571428571427</v>
+        <v>6.6</v>
       </c>
       <c r="H206" s="19"/>
-      <c r="I206" s="19">
-        <v>8</v>
-      </c>
+      <c r="I206" s="19"/>
       <c r="J206" s="19"/>
       <c r="K206" s="19"/>
       <c r="L206" s="19"/>
@@ -10965,29 +10967,29 @@
     </row>
     <row r="207" spans="1:17" ht="15.6">
       <c r="A207" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B207" s="70" t="s">
-        <v>485</v>
+        <v>188</v>
+      </c>
+      <c r="B207" s="65" t="s">
+        <v>449</v>
       </c>
       <c r="C207" s="39" t="s">
         <v>158</v>
       </c>
       <c r="D207" s="19">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E207" s="19">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F207" s="19"/>
       <c r="G207" s="21">
-        <f t="shared" si="15"/>
-        <v>6.2857142857142856</v>
-      </c>
-      <c r="H207" s="19">
-        <v>4</v>
-      </c>
-      <c r="I207" s="19"/>
+        <f>(E207/5)+(F207)+(D207/7)</f>
+        <v>6.5428571428571427</v>
+      </c>
+      <c r="H207" s="19"/>
+      <c r="I207" s="19">
+        <v>8</v>
+      </c>
       <c r="J207" s="19"/>
       <c r="K207" s="19"/>
       <c r="L207" s="19"/>
@@ -10999,31 +11001,29 @@
     </row>
     <row r="208" spans="1:17" ht="15.6">
       <c r="A208" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="B208" s="64" t="s">
-        <v>472</v>
+        <v>93</v>
+      </c>
+      <c r="B208" s="70" t="s">
+        <v>485</v>
       </c>
       <c r="C208" s="39" t="s">
         <v>158</v>
       </c>
       <c r="D208" s="19">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E208" s="19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F208" s="19"/>
       <c r="G208" s="21">
-        <f>(E208/5)+(F208)+(D208/7)</f>
-        <v>5.8285714285714292</v>
+        <f t="shared" si="15"/>
+        <v>6.2857142857142856</v>
       </c>
       <c r="H208" s="19">
-        <v>7</v>
-      </c>
-      <c r="I208" s="19">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I208" s="19"/>
       <c r="J208" s="19"/>
       <c r="K208" s="19"/>
       <c r="L208" s="19"/>
@@ -11034,105 +11034,111 @@
       <c r="Q208" s="28"/>
     </row>
     <row r="209" spans="1:17" ht="15.6">
-      <c r="A209" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="B209" s="63" t="s">
-        <v>389</v>
+      <c r="A209" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B209" s="64" t="s">
+        <v>472</v>
       </c>
       <c r="C209" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="D209" s="19"/>
+      <c r="D209" s="19">
+        <v>31</v>
+      </c>
       <c r="E209" s="19">
-        <v>11</v>
-      </c>
-      <c r="F209" s="19">
-        <v>3</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F209" s="19"/>
       <c r="G209" s="21">
         <f>(E209/5)+(F209)+(D209/7)</f>
-        <v>5.2</v>
+        <v>5.8285714285714292</v>
       </c>
       <c r="H209" s="19">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I209" s="19">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J209" s="19"/>
-      <c r="K209" s="19">
-        <v>6</v>
-      </c>
-      <c r="L209" s="19">
-        <v>6</v>
-      </c>
-      <c r="M209" s="19">
-        <v>6</v>
-      </c>
-      <c r="N209" s="19">
-        <v>6</v>
-      </c>
-      <c r="O209" s="19">
-        <v>6</v>
-      </c>
+      <c r="K209" s="19"/>
+      <c r="L209" s="19"/>
+      <c r="M209" s="19"/>
+      <c r="N209" s="19"/>
+      <c r="O209" s="19"/>
       <c r="P209" s="28"/>
       <c r="Q209" s="28"/>
     </row>
     <row r="210" spans="1:17" ht="15.6">
-      <c r="A210" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B210" s="64" t="s">
-        <v>439</v>
+      <c r="A210" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B210" s="63" t="s">
+        <v>389</v>
       </c>
       <c r="C210" s="39" t="s">
         <v>158</v>
       </c>
       <c r="D210" s="19"/>
-      <c r="E210" s="19"/>
+      <c r="E210" s="19">
+        <v>11</v>
+      </c>
       <c r="F210" s="19">
+        <v>3</v>
+      </c>
+      <c r="G210" s="21">
+        <f>(E210/5)+(F210)+(D210/7)</f>
+        <v>5.2</v>
+      </c>
+      <c r="H210" s="19">
+        <v>11</v>
+      </c>
+      <c r="I210" s="19">
+        <v>11</v>
+      </c>
+      <c r="J210" s="19"/>
+      <c r="K210" s="19">
+        <v>6</v>
+      </c>
+      <c r="L210" s="19">
+        <v>6</v>
+      </c>
+      <c r="M210" s="19">
+        <v>6</v>
+      </c>
+      <c r="N210" s="19">
+        <v>6</v>
+      </c>
+      <c r="O210" s="19">
+        <v>6</v>
+      </c>
+      <c r="P210" s="28"/>
+      <c r="Q210" s="28"/>
+    </row>
+    <row r="211" spans="1:17" ht="15.6">
+      <c r="A211" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B211" s="64" t="s">
+        <v>439</v>
+      </c>
+      <c r="C211" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D211" s="19"/>
+      <c r="E211" s="19"/>
+      <c r="F211" s="19">
         <v>5</v>
       </c>
-      <c r="G210" s="21">
+      <c r="G211" s="21">
         <f t="shared" si="15"/>
         <v>5</v>
       </c>
-      <c r="H210" s="19"/>
-      <c r="I210" s="19"/>
-      <c r="J210" s="19">
-        <v>1</v>
-      </c>
-      <c r="K210" s="19"/>
-      <c r="L210" s="19"/>
-      <c r="M210" s="19"/>
-      <c r="N210" s="19"/>
-      <c r="O210" s="19"/>
-      <c r="P210" s="28"/>
-      <c r="Q210" s="28"/>
-    </row>
-    <row r="211" spans="1:17" ht="15.6">
-      <c r="A211" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="B211" s="63" t="s">
-        <v>393</v>
-      </c>
-      <c r="C211" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="D211" s="19">
-        <v>33</v>
-      </c>
-      <c r="E211" s="19"/>
-      <c r="F211" s="19"/>
-      <c r="G211" s="21">
-        <f>(E211/5)+(F211)+(D211/7)</f>
-        <v>4.7142857142857144</v>
-      </c>
       <c r="H211" s="19"/>
       <c r="I211" s="19"/>
-      <c r="J211" s="19"/>
+      <c r="J211" s="19">
+        <v>1</v>
+      </c>
       <c r="K211" s="19"/>
       <c r="L211" s="19"/>
       <c r="M211" s="19"/>
@@ -11143,29 +11149,25 @@
     </row>
     <row r="212" spans="1:17" ht="15.6">
       <c r="A212" s="5" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="B212" s="63" t="s">
-        <v>470</v>
+        <v>393</v>
       </c>
       <c r="C212" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="D212" s="19"/>
-      <c r="E212" s="19">
-        <v>23</v>
-      </c>
+      <c r="D212" s="19">
+        <v>33</v>
+      </c>
+      <c r="E212" s="19"/>
       <c r="F212" s="19"/>
       <c r="G212" s="21">
         <f>(E212/5)+(F212)+(D212/7)</f>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H212" s="19">
-        <v>13</v>
-      </c>
-      <c r="I212" s="19">
-        <v>10</v>
-      </c>
+        <v>4.7142857142857144</v>
+      </c>
+      <c r="H212" s="19"/>
+      <c r="I212" s="19"/>
       <c r="J212" s="19"/>
       <c r="K212" s="19"/>
       <c r="L212" s="19"/>
@@ -11176,31 +11178,29 @@
       <c r="Q212" s="28"/>
     </row>
     <row r="213" spans="1:17" ht="15.6">
-      <c r="A213" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B213" s="64" t="s">
-        <v>409</v>
+      <c r="A213" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B213" s="63" t="s">
+        <v>470</v>
       </c>
       <c r="C213" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="D213" s="19">
-        <v>15</v>
-      </c>
+      <c r="D213" s="19"/>
       <c r="E213" s="19">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F213" s="19"/>
       <c r="G213" s="21">
-        <f t="shared" si="15"/>
-        <v>4.5428571428571427</v>
+        <f>(E213/5)+(F213)+(D213/7)</f>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H213" s="19">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I213" s="19">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J213" s="19"/>
       <c r="K213" s="19"/>
@@ -11213,31 +11213,31 @@
     </row>
     <row r="214" spans="1:17" ht="15.6">
       <c r="A214" s="4" t="s">
-        <v>566</v>
-      </c>
-      <c r="B214" s="102" t="s">
-        <v>567</v>
+        <v>39</v>
+      </c>
+      <c r="B214" s="64" t="s">
+        <v>409</v>
       </c>
       <c r="C214" s="39" t="s">
         <v>158</v>
       </c>
       <c r="D214" s="19">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E214" s="19">
-        <v>10</v>
-      </c>
-      <c r="F214" s="19">
-        <v>4</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F214" s="19"/>
       <c r="G214" s="21">
         <f t="shared" si="15"/>
-        <v>9.1428571428571423</v>
+        <v>4.5428571428571427</v>
       </c>
       <c r="H214" s="19">
-        <v>10</v>
-      </c>
-      <c r="I214" s="19"/>
+        <v>7</v>
+      </c>
+      <c r="I214" s="19">
+        <v>8</v>
+      </c>
       <c r="J214" s="19"/>
       <c r="K214" s="19"/>
       <c r="L214" s="19"/>

</xml_diff>